<commit_message>
fix bug of repeated indicators (2nd try) and separate threshold unit and values
</commit_message>
<xml_diff>
--- a/data/unsd/countryProfiles/input/CountryProfileBuilder_new.xlsx
+++ b/data/unsd/countryProfiles/input/CountryProfileBuilder_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.GonzalezMorales\Documents\GitHub\FIS4SDGs\data\unsd\countryProfiles\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1B2F3C-461B-4FAD-B1CA-42E7079BA678}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3006E47-9BA8-47A5-AA37-022E6E8DF42A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" xr2:uid="{608E191F-5FEB-4D0E-811F-33218E7FD720}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="376">
   <si>
     <t>SeriesCode</t>
   </si>
@@ -1327,9 +1327,6 @@
   </si>
   <si>
     <t>The proportion of urban population using safely managed sanitation services</t>
-  </si>
-  <si>
-    <t>10  micrograms per cubic metre</t>
   </si>
 </sst>
 </file>
@@ -1713,10 +1710,10 @@
   <dimension ref="A1:Z55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="Y31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y67" sqref="Y67"/>
+      <selection pane="bottomRight" activeCell="Z36" sqref="Z36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -3427,8 +3424,8 @@
       <c r="Y36" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="Z36" s="2" t="s">
-        <v>376</v>
+      <c r="Z36" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="36" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update factBuilder with hub ids
</commit_message>
<xml_diff>
--- a/data/unsd/countryProfiles/input/CountryProfileBuilder_new.xlsx
+++ b/data/unsd/countryProfiles/input/CountryProfileBuilder_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.GonzalezMorales\Documents\GitHub\FIS4SDGs\data\unsd\countryProfiles\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6854F820-9F98-4422-AC03-8E46C6A8FC1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83920B13-6E10-4E9C-8A3A-CE9BA4485976}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11772" xr2:uid="{608E191F-5FEB-4D0E-811F-33218E7FD720}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CountryProfileBuilder!$A$1:$AH$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CountryProfileBuilder!$A$1:$AI$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!#REF!</definedName>
     <definedName name="_xlnm.Extract" localSheetId="1">Sheet1!$A$1</definedName>
   </definedNames>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="424">
   <si>
     <t>SeriesCode</t>
   </si>
@@ -1308,9 +1308,6 @@
     <t>dashboardId</t>
   </si>
   <si>
-    <t>62f44e7da0864b1eb6f9d4bb5f9d2f54</t>
-  </si>
-  <si>
     <r>
       <t>of the population used a "safely managed" sanitation service</t>
     </r>
@@ -1363,6 +1360,150 @@
   </si>
   <si>
     <t>The score of adoption and implementation of national disaster and risk reduction strategies</t>
+  </si>
+  <si>
+    <t>hubId</t>
+  </si>
+  <si>
+    <t>d80b4105e32a4832bbea4e0bd3dcbf40</t>
+  </si>
+  <si>
+    <t>ee9dd63027a442cb9af00d1d289a14e4</t>
+  </si>
+  <si>
+    <t>17d4351d412c4c05a0e45c31f5cc1385</t>
+  </si>
+  <si>
+    <t>f7f1ee3e71f14210a777d25aa95b846c</t>
+  </si>
+  <si>
+    <t>68674946646d4303a8429ca180b14481</t>
+  </si>
+  <si>
+    <t>29b8dbe8209c4966802edf3a38623f2c</t>
+  </si>
+  <si>
+    <t>efe5c0628d4749b38b4be596740e2956</t>
+  </si>
+  <si>
+    <t>97f4c9aba77f4fed8f217784dfdd649f</t>
+  </si>
+  <si>
+    <t>c386199f78d041d5b1c7b5403ed6bc52</t>
+  </si>
+  <si>
+    <t>36ff192d48504b34bbc8af3ff30f565b</t>
+  </si>
+  <si>
+    <t>27d1c1e5ebc6410597603e9bf52829f3</t>
+  </si>
+  <si>
+    <t>b224da3fb5df4cbe83dc8b20de71dc89</t>
+  </si>
+  <si>
+    <t>2f7acf84fdad47d183f7e2041b474e02</t>
+  </si>
+  <si>
+    <t>e061fd67f9f84933addcd27ca6154354</t>
+  </si>
+  <si>
+    <t>254e360b5e434665b99233dd1d6747cb</t>
+  </si>
+  <si>
+    <t>c4bdefff898c4183a01dcdc6d085ff26</t>
+  </si>
+  <si>
+    <t>8bb6d84e7a5a4253ba5dba1c9144439b</t>
+  </si>
+  <si>
+    <t>c87948a7e6ab4aec92abffb70bab4e7c</t>
+  </si>
+  <si>
+    <t>db95089773654b6898ef4af01c440140</t>
+  </si>
+  <si>
+    <t>6d84807ee23f4ddbaf2b9ba0768c8a12</t>
+  </si>
+  <si>
+    <t>961186c499834224bb09e32f68092855</t>
+  </si>
+  <si>
+    <t>bcf2ed2c448a4a3bafe7ea8951d4a259</t>
+  </si>
+  <si>
+    <t>54681bb23185478eb1e01e147bf32f5d</t>
+  </si>
+  <si>
+    <t>359a92a4ce7545a7a6614a31440f9f5a</t>
+  </si>
+  <si>
+    <t>9e748f270b064e76b062cba1d81982a5</t>
+  </si>
+  <si>
+    <t>164c07649d7d4c0fa50ea2175619ba61</t>
+  </si>
+  <si>
+    <t>08f4e15e1afe43d8a9bbeeae7f4bd3ca</t>
+  </si>
+  <si>
+    <t>7794a89241654512bc4117205a9d6d00</t>
+  </si>
+  <si>
+    <t>9fcf31b0eb6b40ddb8a4c963bf78d761</t>
+  </si>
+  <si>
+    <t>50b0017bc20a400e8bfb92da7591a28b</t>
+  </si>
+  <si>
+    <t>1dc5d53ca0834e8da4594e86180cf55e</t>
+  </si>
+  <si>
+    <t>f205b31db8bf44ea9f8d23b41cd4a9a9</t>
+  </si>
+  <si>
+    <t>06bbe00c627d46f884b9caf36413ad97</t>
+  </si>
+  <si>
+    <t>00e65cf61d8042f591c27ddb56d10063</t>
+  </si>
+  <si>
+    <t>e9df4c5818464ca89b1f0cc403897836</t>
+  </si>
+  <si>
+    <t>f0b52ccea69a48b09df3f5fd58e58e84</t>
+  </si>
+  <si>
+    <t>184b20498cbc4f48831c47e5d9433d4c</t>
+  </si>
+  <si>
+    <t>f503b6296a1b48439c57788ac9a10619</t>
+  </si>
+  <si>
+    <t>6e8b1982b7a643b9bb1906a8edfd31a2</t>
+  </si>
+  <si>
+    <t>1e40231c75c64219952a92c61d916452</t>
+  </si>
+  <si>
+    <t>9e7ac88c99e1423abcac29a5f5a3ab28</t>
+  </si>
+  <si>
+    <t>1206e053761f4924869688ab3bb6a53c</t>
+  </si>
+  <si>
+    <t>3a49aa2198544ff5ad4f856f1a71135b</t>
+  </si>
+  <si>
+    <t>6070453223094596870eb5f16996d0bb</t>
+  </si>
+  <si>
+    <t>2220f2631b044c80811e3209baed8871</t>
+  </si>
+  <si>
+    <t>b23f560693c240b29009e570903b5ff2</t>
+  </si>
+  <si>
+    <t>007e996bd74146de86baa15033995ee2</t>
   </si>
 </sst>
 </file>
@@ -1743,31 +1884,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BF65AC-2E6C-4B3F-8D19-434C6AC10D50}">
-  <dimension ref="A1:AA55"/>
+  <dimension ref="A1:AB55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y38" sqref="Y38"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="4" width="5.109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="43.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16" width="7.44140625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="12.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="26" width="22" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="27.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="2" customWidth="1"/>
+    <col min="8" max="9" width="43.6640625" style="2" customWidth="1"/>
+    <col min="10" max="17" width="7.44140625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="12.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="22" style="2" customWidth="1"/>
+    <col min="28" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="36" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>144</v>
       </c>
@@ -1784,73 +1926,76 @@
         <v>142</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="R1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="48" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="48" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1867,40 +2012,40 @@
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G2" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="Q2" s="3">
-        <v>1</v>
-      </c>
       <c r="R2" s="3">
         <v>1</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>8</v>
+      <c r="S2" s="3">
+        <v>1</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="48" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1917,40 +2062,40 @@
         <v>17</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G3" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q3" s="3">
-        <v>1</v>
-      </c>
       <c r="R3" s="3">
         <v>1</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="3">
+        <v>1</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" ht="36" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1967,46 +2112,46 @@
         <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G4" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q4" s="3">
-        <v>1</v>
-      </c>
       <c r="R4" s="3">
         <v>1</v>
       </c>
-      <c r="S4" s="3" t="s">
-        <v>8</v>
+      <c r="S4" s="3">
+        <v>1</v>
       </c>
       <c r="T4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="U4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="Z4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" s="2" t="s">
+      <c r="AA4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -2023,46 +2168,46 @@
         <v>28</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G5" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="R5" s="3">
         <v>0</v>
       </c>
-      <c r="R5" s="3">
-        <v>1</v>
-      </c>
-      <c r="S5" s="3" t="s">
+      <c r="S5" s="3">
+        <v>1</v>
+      </c>
+      <c r="T5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="U5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Z5" s="2" t="s">
+      <c r="AA5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="96" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" ht="96" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -2079,43 +2224,43 @@
         <v>128</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G6" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="R6" s="3">
         <v>0</v>
       </c>
-      <c r="R6" s="3">
-        <v>1</v>
-      </c>
-      <c r="S6" s="3" t="s">
+      <c r="S6" s="3">
+        <v>1</v>
+      </c>
+      <c r="T6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="V6" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="X6" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="Y6" s="2" t="s">
+      <c r="Z6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="AA6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" ht="36" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -2132,40 +2277,40 @@
         <v>57</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G7" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="R7" s="3">
         <v>0</v>
       </c>
-      <c r="R7" s="3">
-        <v>1</v>
-      </c>
-      <c r="S7" s="3" t="s">
+      <c r="S7" s="3">
+        <v>1</v>
+      </c>
+      <c r="T7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="V7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="X7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Y7" s="2" t="s">
+      <c r="Z7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z7" s="2" t="s">
+      <c r="AA7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="36" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -2182,40 +2327,40 @@
         <v>67</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G8" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="R8" s="3">
         <v>0</v>
       </c>
-      <c r="R8" s="3">
-        <v>1</v>
-      </c>
-      <c r="S8" s="3" t="s">
+      <c r="S8" s="3">
+        <v>1</v>
+      </c>
+      <c r="T8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="V8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="Y8" s="2" t="s">
+      <c r="Z8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="AA8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" ht="36" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -2232,37 +2377,37 @@
         <v>76</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G9" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="R9" s="3">
         <v>0</v>
       </c>
-      <c r="R9" s="3">
-        <v>1</v>
-      </c>
-      <c r="S9" s="3" t="s">
+      <c r="S9" s="3">
+        <v>1</v>
+      </c>
+      <c r="T9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="V9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="X9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Y9" s="2" t="s">
+      <c r="Z9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z9" s="2" t="s">
+      <c r="AA9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -2279,43 +2424,43 @@
         <v>79</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G10" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="R10" s="3">
         <v>0</v>
       </c>
-      <c r="R10" s="3">
-        <v>1</v>
-      </c>
-      <c r="S10" s="3" t="s">
+      <c r="S10" s="3">
+        <v>1</v>
+      </c>
+      <c r="T10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U10" s="2" t="s">
+      <c r="V10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="X10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Y10" s="2" t="s">
+      <c r="Z10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z10" s="2" t="s">
+      <c r="AA10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" ht="36" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -2332,37 +2477,37 @@
         <v>82</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G11" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="R11" s="3">
         <v>0</v>
       </c>
-      <c r="R11" s="3">
-        <v>1</v>
-      </c>
-      <c r="S11" s="3" t="s">
+      <c r="S11" s="3">
+        <v>1</v>
+      </c>
+      <c r="T11" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="V11" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="W11" s="2" t="s">
+      <c r="X11" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="Y11" s="2" t="s">
+      <c r="Z11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z11" s="2" t="s">
+      <c r="AA11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" ht="24" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>1</v>
       </c>
@@ -2379,37 +2524,37 @@
         <v>98</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G12" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="R12" s="3">
         <v>0</v>
       </c>
-      <c r="R12" s="3">
-        <v>1</v>
-      </c>
-      <c r="S12" s="3" t="s">
+      <c r="S12" s="3">
+        <v>1</v>
+      </c>
+      <c r="T12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U12" s="2" t="s">
+      <c r="V12" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="W12" s="2" t="s">
+      <c r="X12" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="Y12" s="2" t="s">
+      <c r="Z12" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="Z12" s="2" t="s">
+      <c r="AA12" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" ht="36" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -2426,40 +2571,40 @@
         <v>70</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G13" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="O13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Q13" s="3">
-        <v>1</v>
-      </c>
       <c r="R13" s="3">
         <v>1</v>
       </c>
-      <c r="S13" s="3" t="s">
+      <c r="S13" s="3">
+        <v>1</v>
+      </c>
+      <c r="T13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="U13" s="2" t="s">
+      <c r="V13" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="W13" s="2" t="s">
+      <c r="X13" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="Y13" s="2" t="s">
+      <c r="Z13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z13" s="2" t="s">
+      <c r="AA13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="36" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -2476,37 +2621,37 @@
         <v>105</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G14" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="Q14" s="3">
-        <v>1</v>
-      </c>
       <c r="R14" s="3">
         <v>1</v>
       </c>
-      <c r="S14" s="3" t="s">
+      <c r="S14" s="3">
+        <v>1</v>
+      </c>
+      <c r="T14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U14" s="2" t="s">
+      <c r="V14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="W14" s="2" t="s">
+      <c r="X14" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="Y14" s="2" t="s">
+      <c r="Z14" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="Z14" s="2" t="s">
+      <c r="AA14" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" ht="36" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>1</v>
       </c>
@@ -2523,40 +2668,40 @@
         <v>116</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G15" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="Q15" s="3">
-        <v>1</v>
-      </c>
       <c r="R15" s="3">
         <v>1</v>
       </c>
-      <c r="S15" s="3" t="s">
-        <v>8</v>
+      <c r="S15" s="3">
+        <v>1</v>
       </c>
       <c r="T15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U15" s="2" t="s">
+      <c r="U15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V15" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="W15" s="2" t="s">
+      <c r="X15" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="Y15" s="2" t="s">
+      <c r="Z15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z15" s="2" t="s">
+      <c r="AA15" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="48" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" ht="48" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1</v>
       </c>
@@ -2573,46 +2718,46 @@
         <v>13</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G16" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="L16" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q16" s="3">
-        <v>1</v>
-      </c>
       <c r="R16" s="3">
+        <v>1</v>
+      </c>
+      <c r="S16" s="3">
         <v>2</v>
       </c>
-      <c r="S16" s="3" t="s">
+      <c r="T16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="T16" s="3" t="s">
+      <c r="U16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U16" s="2" t="s">
+      <c r="V16" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="W16" s="2" t="s">
+      <c r="X16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Y16" s="2" t="s">
+      <c r="Z16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Z16" s="2" t="s">
+      <c r="AA16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>1</v>
       </c>
@@ -2629,46 +2774,46 @@
         <v>19</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G17" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q17" s="3">
-        <v>1</v>
-      </c>
       <c r="R17" s="3">
+        <v>1</v>
+      </c>
+      <c r="S17" s="3">
         <v>2</v>
       </c>
-      <c r="S17" s="3" t="s">
+      <c r="T17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="T17" s="3" t="s">
+      <c r="U17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U17" s="2" t="s">
+      <c r="V17" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="W17" s="2" t="s">
+      <c r="X17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Y17" s="2" t="s">
+      <c r="Z17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Z17" s="2" t="s">
+      <c r="AA17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="60" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" ht="60" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>1</v>
       </c>
@@ -2685,40 +2830,40 @@
         <v>130</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G18" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q18" s="3">
+      <c r="R18" s="3">
         <v>0</v>
       </c>
-      <c r="R18" s="3">
+      <c r="S18" s="3">
         <v>2</v>
       </c>
-      <c r="S18" s="3" t="s">
+      <c r="T18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U18" s="2" t="s">
+      <c r="V18" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="W18" s="2" t="s">
+      <c r="X18" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="Y18" s="2" t="s">
+      <c r="Z18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Z18" s="2" t="s">
+      <c r="AA18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="48" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" ht="48" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>1</v>
       </c>
@@ -2735,43 +2880,43 @@
         <v>60</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G19" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="R19" s="3">
         <v>0</v>
       </c>
-      <c r="R19" s="3">
+      <c r="S19" s="3">
         <v>2</v>
       </c>
-      <c r="S19" s="3" t="s">
+      <c r="T19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U19" s="2" t="s">
+      <c r="V19" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="W19" s="2" t="s">
+      <c r="X19" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="Y19" s="2" t="s">
+      <c r="Z19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Z19" s="2" t="s">
+      <c r="AA19" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -2788,40 +2933,40 @@
         <v>64</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G20" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="K20" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="R20" s="3">
         <v>0</v>
       </c>
-      <c r="R20" s="3">
+      <c r="S20" s="3">
         <v>2</v>
       </c>
-      <c r="S20" s="3" t="s">
+      <c r="T20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U20" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="W20" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="Y20" s="2" t="s">
+      <c r="V20" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="X20" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="Z20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Z20" s="2" t="s">
+      <c r="AA20" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" ht="24" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
         <v>6</v>
       </c>
@@ -2835,40 +2980,40 @@
         <v>61</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G21" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="K21" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q21" s="3">
-        <v>1</v>
-      </c>
       <c r="R21" s="3">
+        <v>1</v>
+      </c>
+      <c r="S21" s="3">
         <v>2</v>
       </c>
-      <c r="S21" s="3" t="s">
+      <c r="T21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U21" s="2" t="s">
+      <c r="V21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="W21" s="2" t="s">
+      <c r="X21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="Y21" s="2" t="s">
+      <c r="Z21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Z21" s="2" t="s">
+      <c r="AA21" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="60" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" ht="60" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>1</v>
       </c>
@@ -2885,40 +3030,40 @@
         <v>63</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="R22" s="3">
+        <v>0</v>
+      </c>
+      <c r="S22" s="3">
+        <v>2</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V22" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q22" s="3">
-        <v>0</v>
-      </c>
-      <c r="R22" s="3">
-        <v>2</v>
-      </c>
-      <c r="S22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="U22" s="2" t="s">
+      <c r="X22" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="W22" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="Y22" s="2" t="s">
+      <c r="Z22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Z22" s="2" t="s">
+      <c r="AA22" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" ht="36" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -2935,40 +3080,40 @@
         <v>89</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G23" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="P23" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="Q23" s="3">
+      <c r="R23" s="3">
         <v>0</v>
       </c>
-      <c r="R23" s="3">
+      <c r="S23" s="3">
         <v>2</v>
       </c>
-      <c r="S23" s="3" t="s">
+      <c r="T23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U23" s="2" t="s">
+      <c r="V23" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="W23" s="2" t="s">
+      <c r="X23" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="Y23" s="2" t="s">
+      <c r="Z23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Z23" s="2" t="s">
+      <c r="AA23" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" ht="36" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>1</v>
       </c>
@@ -2985,37 +3130,37 @@
         <v>92</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G24" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="Q24" s="3">
+      <c r="R24" s="3">
         <v>0</v>
       </c>
-      <c r="R24" s="3">
+      <c r="S24" s="3">
         <v>2</v>
       </c>
-      <c r="S24" s="3" t="s">
+      <c r="T24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U24" s="2" t="s">
+      <c r="V24" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="W24" s="2" t="s">
+      <c r="X24" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="Y24" s="2" t="s">
+      <c r="Z24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Z24" s="2" t="s">
+      <c r="AA24" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" ht="36" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>1</v>
       </c>
@@ -3032,40 +3177,40 @@
         <v>111</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G25" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="J25" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="Q25" s="3">
+      <c r="R25" s="3">
         <v>0</v>
       </c>
-      <c r="R25" s="3">
+      <c r="S25" s="3">
         <v>3</v>
       </c>
-      <c r="S25" s="3" t="s">
+      <c r="T25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U25" s="2" t="s">
+      <c r="V25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="V25" s="2" t="s">
+      <c r="W25" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="W25" s="2" t="s">
+      <c r="X25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="X25" s="2" t="s">
+      <c r="Y25" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="48" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" ht="48" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>1</v>
       </c>
@@ -3082,37 +3227,37 @@
         <v>45</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G26" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="N26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q26" s="3">
+      <c r="R26" s="3">
         <v>0</v>
       </c>
-      <c r="R26" s="3">
+      <c r="S26" s="3">
         <v>4</v>
       </c>
-      <c r="U26" s="2" t="s">
+      <c r="V26" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="V26" s="2" t="s">
+      <c r="W26" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="W26" s="2" t="s">
+      <c r="X26" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="X26" s="2" t="s">
+      <c r="Y26" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" ht="36" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>1</v>
       </c>
@@ -3129,37 +3274,37 @@
         <v>48</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G27" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="M27" s="3" t="s">
+      <c r="N27" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q27" s="3">
+      <c r="R27" s="3">
         <v>0</v>
       </c>
-      <c r="R27" s="3">
+      <c r="S27" s="3">
         <v>4</v>
       </c>
-      <c r="U27" s="2" t="s">
+      <c r="V27" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="V27" s="2" t="s">
+      <c r="W27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="W27" s="2" t="s">
+      <c r="X27" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="X27" s="2" t="s">
+      <c r="Y27" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" ht="36" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>1</v>
       </c>
@@ -3176,40 +3321,40 @@
         <v>23</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G28" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="Q28" s="3">
+      <c r="R28" s="3">
         <v>0</v>
       </c>
-      <c r="R28" s="3">
+      <c r="S28" s="3">
         <v>7</v>
-      </c>
-      <c r="S28" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="T28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U28" s="2" t="s">
+      <c r="U28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="W28" s="2" t="s">
+      <c r="X28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Y28" s="2" t="s">
+      <c r="Z28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z28" s="2" t="s">
+      <c r="AA28" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" ht="36" x14ac:dyDescent="0.3">
       <c r="B29" s="2">
         <v>12</v>
       </c>
@@ -3223,34 +3368,34 @@
         <v>210</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G29" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="N29" s="3" t="s">
+      <c r="O29" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Q29" s="3">
-        <v>1</v>
-      </c>
       <c r="R29" s="3">
+        <v>1</v>
+      </c>
+      <c r="S29" s="3">
         <v>7</v>
       </c>
-      <c r="S29" s="3" t="s">
+      <c r="T29" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="U29" s="2" t="s">
+      <c r="V29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="W29" s="2" t="s">
+      <c r="X29" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="48" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" ht="48" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>1</v>
       </c>
@@ -3267,34 +3412,34 @@
         <v>107</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G30" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="M30" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q30" s="3">
-        <v>1</v>
-      </c>
       <c r="R30" s="3">
+        <v>1</v>
+      </c>
+      <c r="S30" s="3">
         <v>7</v>
       </c>
-      <c r="S30" s="3" t="s">
+      <c r="T30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U30" s="2" t="s">
+      <c r="V30" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="W30" s="2" t="s">
+      <c r="X30" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="48" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" ht="48" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>1</v>
       </c>
@@ -3311,34 +3456,34 @@
         <v>109</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G31" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="M31" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q31" s="3">
-        <v>1</v>
-      </c>
       <c r="R31" s="3">
+        <v>1</v>
+      </c>
+      <c r="S31" s="3">
         <v>7</v>
       </c>
-      <c r="S31" s="3" t="s">
+      <c r="T31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U31" s="2" t="s">
+      <c r="V31" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="W31" s="2" t="s">
+      <c r="X31" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" ht="36" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>1</v>
       </c>
@@ -3355,31 +3500,31 @@
         <v>65</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G32" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="Q32" s="3">
+      <c r="R32" s="3">
         <v>0</v>
       </c>
-      <c r="R32" s="3">
+      <c r="S32" s="3">
         <v>8</v>
       </c>
-      <c r="S32" s="3" t="s">
+      <c r="T32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U32" s="2" t="s">
+      <c r="V32" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="W32" s="2" t="s">
+      <c r="X32" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="48" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" ht="48" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>1</v>
       </c>
@@ -3396,31 +3541,31 @@
         <v>103</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G33" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="Q33" s="3">
-        <v>1</v>
-      </c>
       <c r="R33" s="3">
+        <v>1</v>
+      </c>
+      <c r="S33" s="3">
         <v>8</v>
       </c>
-      <c r="S33" s="3" t="s">
+      <c r="T33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U33" s="2" t="s">
+      <c r="V33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="W33" s="2" t="s">
+      <c r="X33" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" ht="24" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>1</v>
       </c>
@@ -3437,40 +3582,40 @@
         <v>84</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G34" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="Q34" s="3">
+      <c r="R34" s="3">
         <v>0</v>
       </c>
-      <c r="R34" s="3">
+      <c r="S34" s="3">
         <v>9</v>
       </c>
-      <c r="S34" s="3" t="s">
+      <c r="T34" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="T34" s="3" t="s">
+      <c r="U34" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U34" s="2" t="s">
+      <c r="V34" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="W34" s="2" t="s">
+      <c r="X34" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="Y34" s="2" t="s">
+      <c r="Z34" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="Z34" s="2" t="s">
+      <c r="AA34" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" ht="24" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>1</v>
       </c>
@@ -3487,40 +3632,40 @@
         <v>132</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G35" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="Q35" s="3">
-        <v>1</v>
-      </c>
       <c r="R35" s="3">
+        <v>1</v>
+      </c>
+      <c r="S35" s="3">
         <v>9</v>
       </c>
-      <c r="S35" s="3" t="s">
+      <c r="T35" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="T35" s="3" t="s">
+      <c r="U35" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U35" s="2" t="s">
+      <c r="V35" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="W35" s="2" t="s">
+      <c r="X35" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="Y35" s="2" t="s">
+      <c r="Z35" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="Z35" s="2" t="s">
+      <c r="AA35" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="72" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>1</v>
       </c>
@@ -3537,43 +3682,43 @@
         <v>94</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G36" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="J36" s="3" t="s">
+      <c r="K36" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q36" s="3">
+      <c r="R36" s="3">
         <v>0</v>
       </c>
-      <c r="R36" s="3">
+      <c r="S36" s="3">
         <v>10</v>
       </c>
-      <c r="S36" s="3" t="s">
+      <c r="T36" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="U36" s="2" t="s">
+      <c r="V36" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="W36" s="2" t="s">
+      <c r="X36" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="Y36" s="2" t="s">
+      <c r="Z36" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="Z36" s="2" t="s">
+      <c r="AA36" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AA36" s="2">
+      <c r="AB36" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" ht="24" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>1</v>
       </c>
@@ -3590,31 +3735,31 @@
         <v>113</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G37" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="Q37" s="3">
+      <c r="R37" s="3">
         <v>0</v>
       </c>
-      <c r="R37" s="3">
+      <c r="S37" s="3">
         <v>11</v>
       </c>
-      <c r="S37" s="3" t="s">
+      <c r="T37" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="U37" s="2" t="s">
+      <c r="V37" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="W37" s="2" t="s">
+      <c r="X37" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="48" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" ht="48" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>1</v>
       </c>
@@ -3628,43 +3773,43 @@
         <v>211</v>
       </c>
       <c r="E38" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="Q38" s="3">
-        <v>1</v>
+      <c r="I38" s="2" t="s">
+        <v>373</v>
       </c>
       <c r="R38" s="3">
         <v>1</v>
       </c>
-      <c r="S38" s="3" t="s">
-        <v>8</v>
+      <c r="S38" s="3">
+        <v>1</v>
       </c>
       <c r="T38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U38" s="2" t="s">
+      <c r="U38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V38" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="X38" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="W38" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="Y38" s="2" t="s">
+      <c r="Z38" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z38" s="2" t="s">
+      <c r="AA38" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" ht="36" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>1</v>
       </c>
@@ -3681,31 +3826,31 @@
         <v>122</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G39" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="Q39" s="3">
+      <c r="R39" s="3">
         <v>0</v>
       </c>
-      <c r="R39" s="3">
+      <c r="S39" s="3">
         <v>12</v>
       </c>
-      <c r="W39" s="2" t="s">
+      <c r="X39" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="Y39" s="2" t="s">
+      <c r="Z39" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="Z39" s="2" t="s">
+      <c r="AA39" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" ht="36" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>1</v>
       </c>
@@ -3722,46 +3867,46 @@
         <v>33</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G40" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="I40" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="J40" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="K40" s="3" t="s">
+      <c r="L40" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q40" s="3">
-        <v>1</v>
-      </c>
       <c r="R40" s="3">
+        <v>1</v>
+      </c>
+      <c r="S40" s="3">
         <v>13</v>
       </c>
-      <c r="S40" s="3" t="s">
+      <c r="T40" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T40" s="3" t="s">
+      <c r="U40" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="U40" s="2" t="s">
+      <c r="V40" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="V40" s="2" t="s">
+      <c r="W40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="W40" s="2" t="s">
+      <c r="X40" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="X40" s="2" t="s">
+      <c r="Y40" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" ht="24" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>1</v>
       </c>
@@ -3778,40 +3923,40 @@
         <v>39</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>40</v>
+        <v>416</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L41" s="3" t="s">
+      <c r="I41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M41" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q41" s="3">
+      <c r="R41" s="3">
         <v>0</v>
       </c>
-      <c r="R41" s="3">
+      <c r="S41" s="3">
         <v>14</v>
       </c>
-      <c r="S41" s="3" t="s">
+      <c r="T41" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="U41" s="2" t="s">
+      <c r="V41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W41" s="2" t="s">
+      <c r="X41" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Y41" s="2" t="s">
+      <c r="Z41" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z41" s="2" t="s">
+      <c r="AA41" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" ht="24" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>1</v>
       </c>
@@ -3828,43 +3973,43 @@
         <v>118</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G42" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="I42" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="P42" s="3" t="s">
+      <c r="Q42" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="Q42" s="3">
+      <c r="R42" s="3">
         <v>0</v>
       </c>
-      <c r="R42" s="3">
+      <c r="S42" s="3">
         <v>15</v>
       </c>
-      <c r="S42" s="3" t="s">
+      <c r="T42" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="T42" s="3" t="s">
+      <c r="U42" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U42" s="2" t="s">
+      <c r="V42" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="W42" s="2" t="s">
+      <c r="X42" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="Y42" s="2" t="s">
+      <c r="Z42" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Z42" s="2" t="s">
+      <c r="AA42" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="48" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" ht="48" x14ac:dyDescent="0.3">
       <c r="B43" s="2">
         <v>2</v>
       </c>
@@ -3878,43 +4023,43 @@
         <v>22</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G43" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="J43" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="Q43" s="3">
-        <v>1</v>
-      </c>
       <c r="R43" s="3">
         <v>1</v>
       </c>
-      <c r="S43" s="3" t="s">
-        <v>8</v>
+      <c r="S43" s="3">
+        <v>1</v>
       </c>
       <c r="T43" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U43" s="2" t="s">
+      <c r="U43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V43" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="W43" s="2" t="s">
+      <c r="X43" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="Y43" s="2" t="s">
+      <c r="Z43" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z43" s="2" t="s">
+      <c r="AA43" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:27" ht="24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" ht="24" x14ac:dyDescent="0.3">
       <c r="B44" s="2">
         <v>3</v>
       </c>
@@ -3928,31 +4073,31 @@
         <v>44</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>167</v>
+        <v>419</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="Q44" s="3">
-        <v>1</v>
+      <c r="I44" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="R44" s="3">
+        <v>1</v>
+      </c>
+      <c r="S44" s="3">
         <v>11</v>
       </c>
-      <c r="S44" s="3" t="s">
+      <c r="T44" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="U44" s="2" t="s">
+      <c r="V44" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="W44" s="2" t="s">
+      <c r="X44" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" ht="24" x14ac:dyDescent="0.3">
       <c r="B45" s="2">
         <v>3</v>
       </c>
@@ -3966,31 +4111,31 @@
         <v>38</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>164</v>
+        <v>420</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="Q45" s="3">
-        <v>1</v>
+      <c r="I45" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="R45" s="3">
+        <v>1</v>
+      </c>
+      <c r="S45" s="3">
         <v>11</v>
       </c>
-      <c r="S45" s="3" t="s">
+      <c r="T45" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="U45" s="2" t="s">
+      <c r="V45" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="W45" s="2" t="s">
+      <c r="X45" s="2" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" ht="36" x14ac:dyDescent="0.3">
       <c r="B46" s="2">
         <v>4</v>
       </c>
@@ -4004,40 +4149,40 @@
         <v>50</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G46" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="I46" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M46" s="3" t="s">
+      <c r="N46" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q46" s="3">
+      <c r="R46" s="3">
         <v>0</v>
       </c>
-      <c r="U46" s="2" t="s">
+      <c r="V46" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="V46" s="2" t="s">
+      <c r="W46" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="W46" s="2" t="s">
+      <c r="X46" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="X46" s="2" t="s">
+      <c r="Y46" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="Y46" s="2" t="s">
+      <c r="Z46" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Z46" s="2" t="s">
+      <c r="AA46" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" ht="24" x14ac:dyDescent="0.3">
       <c r="B47" s="2">
         <v>5</v>
       </c>
@@ -4051,34 +4196,34 @@
         <v>56</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G47" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="I47" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="K47" s="3" t="s">
+      <c r="L47" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="Q47" s="3">
+      <c r="R47" s="3">
         <v>0</v>
       </c>
-      <c r="R47" s="3">
+      <c r="S47" s="3">
         <v>8</v>
       </c>
-      <c r="S47" s="3" t="s">
+      <c r="T47" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U47" s="2" t="s">
+      <c r="V47" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="W47" s="2" t="s">
+      <c r="X47" s="2" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" ht="36" x14ac:dyDescent="0.3">
       <c r="B48" s="2">
         <v>6</v>
       </c>
@@ -4092,43 +4237,43 @@
         <v>61</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G48" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="I48" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="J48" s="3" t="s">
+      <c r="K48" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="Q48" s="3">
-        <v>1</v>
-      </c>
       <c r="R48" s="3">
         <v>1</v>
       </c>
-      <c r="S48" s="3" t="s">
-        <v>8</v>
+      <c r="S48" s="3">
+        <v>1</v>
       </c>
       <c r="T48" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U48" s="2" t="s">
+      <c r="U48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V48" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="W48" s="2" t="s">
+      <c r="X48" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="Y48" s="2" t="s">
+      <c r="Z48" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z48" s="2" t="s">
+      <c r="AA48" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="2:26" ht="36" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:27" ht="36" x14ac:dyDescent="0.3">
       <c r="B49" s="2">
         <v>6</v>
       </c>
@@ -4142,43 +4287,43 @@
         <v>61</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G49" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="J49" s="3" t="s">
+      <c r="K49" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="Q49" s="3">
-        <v>1</v>
-      </c>
       <c r="R49" s="3">
         <v>1</v>
       </c>
-      <c r="S49" s="3" t="s">
-        <v>8</v>
+      <c r="S49" s="3">
+        <v>1</v>
       </c>
       <c r="T49" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U49" s="2" t="s">
+      <c r="U49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V49" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="W49" s="2" t="s">
+      <c r="X49" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="Y49" s="2" t="s">
+      <c r="Z49" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z49" s="2" t="s">
+      <c r="AA49" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="2:26" ht="48" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:27" ht="48" x14ac:dyDescent="0.3">
       <c r="B50" s="2">
         <v>6</v>
       </c>
@@ -4192,43 +4337,43 @@
         <v>63</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G50" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="I50" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="J50" s="3" t="s">
+      <c r="K50" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="Q50" s="3">
+      <c r="R50" s="3">
         <v>0</v>
       </c>
-      <c r="R50" s="3">
-        <v>1</v>
-      </c>
-      <c r="S50" s="3" t="s">
-        <v>8</v>
+      <c r="S50" s="3">
+        <v>1</v>
       </c>
       <c r="T50" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U50" s="2" t="s">
+      <c r="U50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V50" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="W50" s="2" t="s">
+      <c r="X50" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="Y50" s="2" t="s">
+      <c r="Z50" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z50" s="2" t="s">
+      <c r="AA50" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="2:26" ht="48" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:27" ht="48" x14ac:dyDescent="0.3">
       <c r="B51" s="2">
         <v>6</v>
       </c>
@@ -4242,43 +4387,43 @@
         <v>63</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G51" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="I51" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="J51" s="3" t="s">
+      <c r="K51" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="Q51" s="3">
+      <c r="R51" s="3">
         <v>0</v>
       </c>
-      <c r="R51" s="3">
-        <v>1</v>
-      </c>
-      <c r="S51" s="3" t="s">
-        <v>8</v>
+      <c r="S51" s="3">
+        <v>1</v>
       </c>
       <c r="T51" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U51" s="2" t="s">
+      <c r="U51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V51" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="W51" s="2" t="s">
+      <c r="X51" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="Y51" s="2" t="s">
+      <c r="Z51" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z51" s="2" t="s">
+      <c r="AA51" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="2:26" ht="24" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:27" ht="24" x14ac:dyDescent="0.3">
       <c r="B52" s="2">
         <v>8</v>
       </c>
@@ -4292,25 +4437,25 @@
         <v>79</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G52" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="I52" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="I52" s="3" t="s">
+      <c r="J52" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="K52" s="3" t="s">
+      <c r="L52" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="Q52" s="3">
+      <c r="R52" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:26" ht="24" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:27" ht="24" x14ac:dyDescent="0.3">
       <c r="B53" s="2">
         <v>8</v>
       </c>
@@ -4324,25 +4469,25 @@
         <v>79</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G53" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="H53" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="I53" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="I53" s="3" t="s">
+      <c r="J53" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="K53" s="3" t="s">
+      <c r="L53" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="Q53" s="3">
+      <c r="R53" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:26" ht="24" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B54" s="2">
         <v>8</v>
       </c>
@@ -4356,25 +4501,25 @@
         <v>79</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G54" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="H54" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="I54" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="I54" s="3" t="s">
+      <c r="J54" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="K54" s="3" t="s">
+      <c r="L54" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="Q54" s="3">
+      <c r="R54" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:26" ht="24" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:27" ht="24" x14ac:dyDescent="0.3">
       <c r="B55" s="2">
         <v>17</v>
       </c>
@@ -4388,21 +4533,21 @@
         <v>126</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G55" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="I55" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="Q55" s="3">
+      <c r="R55" s="3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Z55">
-    <sortCondition ref="R2:R55"/>
+  <sortState ref="A2:AA55">
+    <sortCondition ref="S2:S55"/>
     <sortCondition ref="B2:B55"/>
     <sortCondition ref="C2:C55"/>
     <sortCondition ref="D2:D55"/>

</xml_diff>